<commit_message>
support sending message to other client.
</commit_message>
<xml_diff>
--- a/doc/长链协议.xlsx
+++ b/doc/长链协议.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/git_repos/im-demo/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E18074-16BA-4142-9C47-C86D18BBE126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CDCC9-DDB1-3041-9F85-B4F21C996242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35600" yWindow="1720" windowWidth="33600" windowHeight="19440" xr2:uid="{231F5A49-B131-B747-841D-0C1C63A81422}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>序号</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>{"type":"business_ack","msgId":"xxxxxxxxxxxxxxxxxxxx"}</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>{"senderId":123,"receiverId":234,"content":"xxx"}</t>
+  </si>
+  <si>
+    <t>{"type":"business","msgId":"xxxxxxxxxxxxxxxxxxxx","subType":"text", "content":"json"}</t>
   </si>
 </sst>
 </file>
@@ -549,7 +558,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1"/>
@@ -558,7 +567,7 @@
     <col min="2" max="2" width="15.83203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="43.1640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="94.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="100.6640625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
@@ -626,7 +635,9 @@
       <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="38">
       <c r="A5" s="6">
@@ -655,26 +666,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9111DD-0CEF-8447-B098-00F0AC8606A6}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="85.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14" style="10" customWidth="1"/>
+    <col min="3" max="3" width="85.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="25" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25" customHeight="1">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>